<commit_message>
Añadidos indicadores de medios puntos, logica para procesarlos, y sql de dim_dates y dim_positions
</commit_message>
<xml_diff>
--- a/Excels/data/2008.xlsx
+++ b/Excels/data/2008.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zaka\Desktop\MOTOGP\Excels\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576B262D-E91E-4F37-BCFA-24A08A9FE548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A66144-1D57-4247-AD37-3F824B45A25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="802" activeTab="10" xr2:uid="{8FC9DF12-B6A5-4483-8CF8-5D33A3FDBE78}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="18075" windowHeight="12255" tabRatio="802" firstSheet="3" activeTab="10" xr2:uid="{8FC9DF12-B6A5-4483-8CF8-5D33A3FDBE78}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="2" r:id="rId1"/>
@@ -1796,12 +1796,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5586,8 +5585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F448AE77-19F1-4579-9E7B-C6EC0030917C}">
   <dimension ref="A1:AA93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94:B98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6674,7 +6673,7 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="2" t="s">
         <v>504</v>
       </c>
       <c r="B19" t="s">

</xml_diff>